<commit_message>
Restrict report to admin only
</commit_message>
<xml_diff>
--- a/static/slos.xlsx
+++ b/static/slos.xlsx
@@ -12,16 +12,22 @@
     <sheet name="22333" sheetId="3" r:id="rId3"/>
     <sheet name="34509" sheetId="4" r:id="rId4"/>
     <sheet name="44444" sheetId="5" r:id="rId5"/>
-    <sheet name="66849" sheetId="6" r:id="rId6"/>
-    <sheet name="86567" sheetId="7" r:id="rId7"/>
-    <sheet name="92874" sheetId="8" r:id="rId8"/>
+    <sheet name="86567" sheetId="6" r:id="rId6"/>
+    <sheet name="86639" sheetId="7" r:id="rId7"/>
+    <sheet name="86681" sheetId="8" r:id="rId8"/>
+    <sheet name="86728" sheetId="9" r:id="rId9"/>
+    <sheet name="86729" sheetId="10" r:id="rId10"/>
+    <sheet name="86756" sheetId="11" r:id="rId11"/>
+    <sheet name="87123" sheetId="12" r:id="rId12"/>
+    <sheet name="87361" sheetId="13" r:id="rId13"/>
+    <sheet name="92874" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="96">
   <si>
     <t>12344</t>
   </si>
@@ -74,9 +80,18 @@
     <t>983111123</t>
   </si>
   <si>
+    <t>983111234</t>
+  </si>
+  <si>
+    <t>983456321</t>
+  </si>
+  <si>
     <t>22333</t>
   </si>
   <si>
+    <t>983087652</t>
+  </si>
+  <si>
     <t>34509</t>
   </si>
   <si>
@@ -104,19 +119,178 @@
     <t>987984958</t>
   </si>
   <si>
-    <t>66849</t>
-  </si>
-  <si>
-    <t>03 : Design, implement, and administer effective IT solutions based on user needs.</t>
-  </si>
-  <si>
-    <t>Design an effective IT solution based on user requirements.</t>
-  </si>
-  <si>
-    <t>Implement and administer an effective IT solution based on user requirements.</t>
-  </si>
-  <si>
-    <t>983087653</t>
+    <t>86567</t>
+  </si>
+  <si>
+    <t>06 : Identify and apply IT methods used to protect the confidentiality, integrity, and availability of information and its delivery systems.</t>
+  </si>
+  <si>
+    <t>Demonstrate comprehension of the Confidentiality, Integrity, and Availability of Information Systems</t>
+  </si>
+  <si>
+    <t>Analyze the Confidentiality, Integrity, and Availability of    an information system</t>
+  </si>
+  <si>
+    <t>Evaluate the Confidentiality, Integrity, and Availability of an information system.</t>
+  </si>
+  <si>
+    <t>121301291</t>
+  </si>
+  <si>
+    <t>987987958</t>
+  </si>
+  <si>
+    <t>86639</t>
+  </si>
+  <si>
+    <t>02 : Define, analyze and apply information system requirements in local and global environments.</t>
+  </si>
+  <si>
+    <t>Demonstrate essential knowledge of information system requirements</t>
+  </si>
+  <si>
+    <t>Analyze and develop appropriate information systems requirements for the given problem</t>
+  </si>
+  <si>
+    <t>Evaluate final product based upon stated requirements</t>
+  </si>
+  <si>
+    <t>101010101</t>
+  </si>
+  <si>
+    <t>983248426</t>
+  </si>
+  <si>
+    <t>983960609</t>
+  </si>
+  <si>
+    <t>86681</t>
+  </si>
+  <si>
+    <t>04 : Demonstrate	and	use	appropriate	project	management methods in the creation of an effective IT project plan.</t>
+  </si>
+  <si>
+    <t>Apply the nine knowledge areas in project management (integration, scope, time, cost,quality, risk, communication, human resources,and procurement) in the creation of an effective IT project plan.</t>
+  </si>
+  <si>
+    <t>Apply the five project management processes(initiation, planning, executing, controlling andmonitoring, and closing) in the creation of an effective IT project plan.</t>
+  </si>
+  <si>
+    <t>983195786</t>
+  </si>
+  <si>
+    <t>983198957</t>
+  </si>
+  <si>
+    <t>983255123</t>
+  </si>
+  <si>
+    <t>983785123</t>
+  </si>
+  <si>
+    <t>86728</t>
+  </si>
+  <si>
+    <t>07 : Identify and incorporate relevant ethical, legal, security,	and	social issues in a technology environment.</t>
+  </si>
+  <si>
+    <t>Identify ethical, legal, security and social issues in information technology.</t>
+  </si>
+  <si>
+    <t>Incorporate ethical, legal, security, and social solutions to identified issues in information technology.</t>
+  </si>
+  <si>
+    <t>Evaluate the incorporation of ethical, legal, security,and social issues and solutions in information technology.</t>
+  </si>
+  <si>
+    <t>86729</t>
+  </si>
+  <si>
+    <t>983689881</t>
+  </si>
+  <si>
+    <t>983689887</t>
+  </si>
+  <si>
+    <t>86756</t>
+  </si>
+  <si>
+    <t>987954654</t>
+  </si>
+  <si>
+    <t>987954663</t>
+  </si>
+  <si>
+    <t>547897878</t>
+  </si>
+  <si>
+    <t>08 : Work effectively in	teams to develop IT	based solutions.</t>
+  </si>
+  <si>
+    <t>Contributes to the team project/work</t>
+  </si>
+  <si>
+    <t>Shows responsibility in performing tasks</t>
+  </si>
+  <si>
+    <t>Values other team members</t>
+  </si>
+  <si>
+    <t>87123</t>
+  </si>
+  <si>
+    <t>983015746</t>
+  </si>
+  <si>
+    <t>983040111</t>
+  </si>
+  <si>
+    <t>983055241</t>
+  </si>
+  <si>
+    <t>983084838</t>
+  </si>
+  <si>
+    <t>983108030</t>
+  </si>
+  <si>
+    <t>983169492</t>
+  </si>
+  <si>
+    <t>983221368</t>
+  </si>
+  <si>
+    <t>983310259</t>
+  </si>
+  <si>
+    <t>983366853</t>
+  </si>
+  <si>
+    <t>983373470</t>
+  </si>
+  <si>
+    <t>983025784</t>
+  </si>
+  <si>
+    <t>983058907</t>
+  </si>
+  <si>
+    <t>983302537</t>
+  </si>
+  <si>
+    <t>10 : Recognize the need for	lifelong professional development.</t>
+  </si>
+  <si>
+    <t>Identify the importance of professional development.</t>
+  </si>
+  <si>
+    <t>Analyze the different avenues for professional development.</t>
+  </si>
+  <si>
+    <t>. Create a plan to achieve professional development.</t>
+  </si>
+  <si>
+    <t>87361</t>
   </si>
   <si>
     <t>09 :  Communicate effectively both orally and in	writing.</t>
@@ -134,25 +308,13 @@
     <t>Speaks using good communication skills.</t>
   </si>
   <si>
-    <t>86567</t>
-  </si>
-  <si>
-    <t>06 : Identify and apply IT methods used to protect the confidentiality, integrity, and availability of information and its delivery systems.</t>
-  </si>
-  <si>
-    <t>Demonstrate comprehension of the Confidentiality, Integrity, and Availability of Information Systems</t>
-  </si>
-  <si>
-    <t>Analyze the Confidentiality, Integrity, and Availability of    an information system</t>
-  </si>
-  <si>
-    <t>Evaluate the Confidentiality, Integrity, and Availability of an information system.</t>
-  </si>
-  <si>
-    <t>121301291</t>
+    <t>983158776</t>
   </si>
   <si>
     <t>92874</t>
+  </si>
+  <si>
+    <t>983126438</t>
   </si>
 </sst>
 </file>
@@ -639,9 +801,1962 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C14">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D14">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E14">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E83"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>11</v>
+      </c>
+      <c r="E21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="C22">
+        <v>0.8181818181818181</v>
+      </c>
+      <c r="D22">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="E22">
+        <v>0.9090909090909092</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56">
+        <v>22</v>
+      </c>
+      <c r="C56">
+        <v>22</v>
+      </c>
+      <c r="D56">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="C57">
+        <v>0.6818181818181818</v>
+      </c>
+      <c r="D57">
+        <v>0.9545454545454545</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>80</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="C74">
+        <v>3</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>84</v>
+      </c>
+      <c r="C76" t="s">
+        <v>85</v>
+      </c>
+      <c r="D76" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <v>4</v>
+      </c>
+      <c r="D77">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <v>8</v>
+      </c>
+      <c r="D78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82">
+        <v>13</v>
+      </c>
+      <c r="C82">
+        <v>13</v>
+      </c>
+      <c r="D82">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>0.9230769230769231</v>
+      </c>
+      <c r="D83">
+        <v>0.8461538461538463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -706,122 +2821,156 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0.25</v>
+      </c>
+      <c r="D15">
         <v>0.5</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
+      <c r="E15">
         <v>1</v>
       </c>
     </row>
@@ -832,7 +2981,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -840,7 +2989,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -863,43 +3012,43 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -916,7 +3065,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -933,52 +3082,69 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <v>0</v>
       </c>
     </row>
@@ -997,7 +3163,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1022,7 +3188,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1039,7 +3205,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1056,7 +3222,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1073,7 +3239,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1222,7 +3388,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1247,7 +3413,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1264,7 +3430,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1281,7 +3447,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1422,317 +3588,158 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +3749,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1778,63 +3785,63 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1842,44 +3849,72 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
+      <c r="B14">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="C14">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1889,55 +3924,202 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.75</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1950,11 +4132,8 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1967,11 +4146,8 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1984,11 +4160,8 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2001,11 +4174,8 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2018,11 +4188,8 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2033,9 +4200,6 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add course number to REST api
</commit_message>
<xml_diff>
--- a/static/slos.xlsx
+++ b/static/slos.xlsx
@@ -12,22 +12,22 @@
     <sheet name="22333" sheetId="3" r:id="rId3"/>
     <sheet name="34509" sheetId="4" r:id="rId4"/>
     <sheet name="44444" sheetId="5" r:id="rId5"/>
-    <sheet name="86567" sheetId="6" r:id="rId6"/>
-    <sheet name="86639" sheetId="7" r:id="rId7"/>
-    <sheet name="86681" sheetId="8" r:id="rId8"/>
-    <sheet name="86728" sheetId="9" r:id="rId9"/>
-    <sheet name="86729" sheetId="10" r:id="rId10"/>
-    <sheet name="86756" sheetId="11" r:id="rId11"/>
-    <sheet name="87123" sheetId="12" r:id="rId12"/>
-    <sheet name="87361" sheetId="13" r:id="rId13"/>
-    <sheet name="92874" sheetId="14" r:id="rId14"/>
+    <sheet name="54321" sheetId="6" r:id="rId6"/>
+    <sheet name="86567" sheetId="7" r:id="rId7"/>
+    <sheet name="86639" sheetId="8" r:id="rId8"/>
+    <sheet name="86681" sheetId="9" r:id="rId9"/>
+    <sheet name="86728" sheetId="10" r:id="rId10"/>
+    <sheet name="86729" sheetId="11" r:id="rId11"/>
+    <sheet name="86756" sheetId="12" r:id="rId12"/>
+    <sheet name="87123" sheetId="13" r:id="rId13"/>
+    <sheet name="87361" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="99">
   <si>
     <t>12344</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Evaluate an Information System</t>
   </si>
   <si>
-    <t>Number of students who scored...</t>
-  </si>
-  <si>
     <t>Exemplary</t>
   </si>
   <si>
@@ -74,49 +71,97 @@
     <t>12345</t>
   </si>
   <si>
-    <t>983774598</t>
-  </si>
-  <si>
-    <t>983111123</t>
-  </si>
-  <si>
-    <t>983111234</t>
-  </si>
-  <si>
-    <t>983456321</t>
+    <t>983774598 George, Trisha</t>
+  </si>
+  <si>
+    <t>983111123 Lee, John</t>
+  </si>
+  <si>
+    <t>983111234 Erok, Kero</t>
+  </si>
+  <si>
+    <t>983456321 Erok Sr., Kero</t>
   </si>
   <si>
     <t>22333</t>
   </si>
   <si>
-    <t>983087652</t>
+    <t>983087652 jones, mark</t>
   </si>
   <si>
     <t>34509</t>
   </si>
   <si>
-    <t>668846546</t>
-  </si>
-  <si>
-    <t>978798321</t>
-  </si>
-  <si>
-    <t>981263256</t>
-  </si>
-  <si>
-    <t>989795159</t>
+    <t>668846546 Hancock, John</t>
+  </si>
+  <si>
+    <t>978798321 Jefferson, Thomas</t>
+  </si>
+  <si>
+    <t>981263256 Hamilton, Alexander</t>
   </si>
   <si>
     <t>44444</t>
   </si>
   <si>
-    <t>983028944</t>
-  </si>
-  <si>
-    <t>987984566</t>
-  </si>
-  <si>
-    <t>987984958</t>
+    <t>983028944 beaty, mark</t>
+  </si>
+  <si>
+    <t>987984566 Buffett, Warren</t>
+  </si>
+  <si>
+    <t>987984958 James, David</t>
+  </si>
+  <si>
+    <t>54321</t>
+  </si>
+  <si>
+    <t>07 : Identify and incorporate relevant ethical, legal, security,	and	social issues in a technology environment.</t>
+  </si>
+  <si>
+    <t>Identify ethical, legal, security and social issues in information technology.</t>
+  </si>
+  <si>
+    <t>Incorporate ethical, legal, security, and social solutions to identified issues in information technology.</t>
+  </si>
+  <si>
+    <t>Evaluate the incorporation of ethical, legal, security,and social issues and solutions in information technology.</t>
+  </si>
+  <si>
+    <t>983000001 Dope, Joe</t>
+  </si>
+  <si>
+    <t>983098765 Bunny, Bugs</t>
+  </si>
+  <si>
+    <t>983111222 Spielburg, Stephen</t>
+  </si>
+  <si>
+    <t>983312465 Ketchum, Ash</t>
+  </si>
+  <si>
+    <t>983333000 8, BB-</t>
+  </si>
+  <si>
+    <t>983909076 Duck, Daffy</t>
+  </si>
+  <si>
+    <t>983983983 983, 983</t>
+  </si>
+  <si>
+    <t>09 :  Communicate effectively both orally and in	writing.</t>
+  </si>
+  <si>
+    <t>Writing fully addresses the assignment and is well organized, and easy to understand</t>
+  </si>
+  <si>
+    <t>Writes sentences that are grammatically correct.</t>
+  </si>
+  <si>
+    <t>Demonstrates an understanding of the material and conveys completeness.</t>
+  </si>
+  <si>
+    <t>Speaks using good communication skills.</t>
   </si>
   <si>
     <t>86567</t>
@@ -134,10 +179,7 @@
     <t>Evaluate the Confidentiality, Integrity, and Availability of an information system.</t>
   </si>
   <si>
-    <t>121301291</t>
-  </si>
-  <si>
-    <t>987987958</t>
+    <t>121301291 Flint, Gregory</t>
   </si>
   <si>
     <t>86639</t>
@@ -155,13 +197,13 @@
     <t>Evaluate final product based upon stated requirements</t>
   </si>
   <si>
-    <t>101010101</t>
-  </si>
-  <si>
-    <t>983248426</t>
-  </si>
-  <si>
-    <t>983960609</t>
+    <t xml:space="preserve">101010101 Cohen, Tarik </t>
+  </si>
+  <si>
+    <t xml:space="preserve">983248426 Trubisky, Mitchell </t>
+  </si>
+  <si>
+    <t xml:space="preserve">983960609 Howard, Jordan </t>
   </si>
   <si>
     <t>86681</t>
@@ -176,52 +218,40 @@
     <t>Apply the five project management processes(initiation, planning, executing, controlling andmonitoring, and closing) in the creation of an effective IT project plan.</t>
   </si>
   <si>
-    <t>983195786</t>
-  </si>
-  <si>
-    <t>983198957</t>
-  </si>
-  <si>
-    <t>983255123</t>
-  </si>
-  <si>
-    <t>983785123</t>
+    <t xml:space="preserve">983195786 Jeter, Derek </t>
+  </si>
+  <si>
+    <t xml:space="preserve">983198957 Bryant, Kris </t>
+  </si>
+  <si>
+    <t>983255123 Rizzo, Antony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">983785123 Suzuki, Ichiro </t>
   </si>
   <si>
     <t>86728</t>
   </si>
   <si>
-    <t>07 : Identify and incorporate relevant ethical, legal, security,	and	social issues in a technology environment.</t>
-  </si>
-  <si>
-    <t>Identify ethical, legal, security and social issues in information technology.</t>
-  </si>
-  <si>
-    <t>Incorporate ethical, legal, security, and social solutions to identified issues in information technology.</t>
-  </si>
-  <si>
-    <t>Evaluate the incorporation of ethical, legal, security,and social issues and solutions in information technology.</t>
-  </si>
-  <si>
     <t>86729</t>
   </si>
   <si>
-    <t>983689881</t>
-  </si>
-  <si>
-    <t>983689887</t>
+    <t>983689881 Smith, John</t>
+  </si>
+  <si>
+    <t>983689887 Rodriguez, Alex</t>
   </si>
   <si>
     <t>86756</t>
   </si>
   <si>
-    <t>987954654</t>
-  </si>
-  <si>
-    <t>987954663</t>
-  </si>
-  <si>
-    <t>547897878</t>
+    <t>987954654 Katie, Markham</t>
+  </si>
+  <si>
+    <t>987954663 Gregory, Joel</t>
+  </si>
+  <si>
+    <t>547897878 Smith, John</t>
   </si>
   <si>
     <t>08 : Work effectively in	teams to develop IT	based solutions.</t>
@@ -239,43 +269,43 @@
     <t>87123</t>
   </si>
   <si>
-    <t>983015746</t>
-  </si>
-  <si>
-    <t>983040111</t>
-  </si>
-  <si>
-    <t>983055241</t>
-  </si>
-  <si>
-    <t>983084838</t>
-  </si>
-  <si>
-    <t>983108030</t>
-  </si>
-  <si>
-    <t>983169492</t>
-  </si>
-  <si>
-    <t>983221368</t>
-  </si>
-  <si>
-    <t>983310259</t>
-  </si>
-  <si>
-    <t>983366853</t>
-  </si>
-  <si>
-    <t>983373470</t>
-  </si>
-  <si>
-    <t>983025784</t>
-  </si>
-  <si>
-    <t>983058907</t>
-  </si>
-  <si>
-    <t>983302537</t>
+    <t>983015746  Caratini, Victor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">983040111 Pena, Felix </t>
+  </si>
+  <si>
+    <t>983055241  Happ, Ian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">983084838 Montgomery, Mike </t>
+  </si>
+  <si>
+    <t xml:space="preserve">983108030 Bryant, Kris </t>
+  </si>
+  <si>
+    <t xml:space="preserve">983169492 Martin, Leonys </t>
+  </si>
+  <si>
+    <t xml:space="preserve">983221368 Arrieta, Jake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">983310259 Duensing, Brian </t>
+  </si>
+  <si>
+    <t>983366853  Almora Jr., Albert</t>
+  </si>
+  <si>
+    <t>983373470 La Stella, Tommy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">983025784 Grimm, Justin </t>
+  </si>
+  <si>
+    <t>983058907  Maples, Dillon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">983302537 Contreras, Willson </t>
   </si>
   <si>
     <t>10 : Recognize the need for	lifelong professional development.</t>
@@ -293,36 +323,26 @@
     <t>87361</t>
   </si>
   <si>
-    <t>09 :  Communicate effectively both orally and in	writing.</t>
-  </si>
-  <si>
-    <t>Writing fully addresses the assignment and is well organized, and easy to understand</t>
-  </si>
-  <si>
-    <t>Writes sentences that are grammatically correct.</t>
-  </si>
-  <si>
-    <t>Demonstrates an understanding of the material and conveys completeness.</t>
-  </si>
-  <si>
-    <t>Speaks using good communication skills.</t>
-  </si>
-  <si>
-    <t>983158776</t>
-  </si>
-  <si>
-    <t>92874</t>
-  </si>
-  <si>
-    <t>983126438</t>
+    <t xml:space="preserve">983158776 Rose, Derrick </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -350,8 +370,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,39 +686,36 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -713,7 +732,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -730,7 +749,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -747,7 +766,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -764,7 +783,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -781,18 +800,18 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
         <v>0</v>
       </c>
     </row>
@@ -802,6 +821,136 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -811,29 +960,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -847,7 +996,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -860,22 +1009,19 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -889,7 +1035,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -903,7 +1049,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -917,7 +1063,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -931,7 +1077,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -945,15 +1091,15 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
         <v>1</v>
       </c>
     </row>
@@ -962,7 +1108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
@@ -972,7 +1118,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -982,22 +1128,22 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1014,7 +1160,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1031,7 +1177,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1047,25 +1193,22 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1082,7 +1225,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1099,7 +1242,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1116,7 +1259,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1133,7 +1276,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1150,46 +1293,46 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
         <v>0.6666666666666666</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>0.3333333333333333</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.6666666666666666</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
+      <c r="B18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -1203,7 +1346,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1217,7 +1360,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -1230,22 +1373,19 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>68</v>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1259,7 +1399,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1273,7 +1413,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1287,7 +1427,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -1301,7 +1441,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1315,15 +1455,15 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="B30" s="2">
         <v>0.6666666666666666</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
         <v>0.6666666666666666</v>
       </c>
     </row>
@@ -1332,7 +1472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E83"/>
   <sheetViews>
@@ -1342,7 +1482,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1352,22 +1492,22 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1384,7 +1524,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1401,7 +1541,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1418,7 +1558,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1435,7 +1575,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1452,7 +1592,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1469,7 +1609,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -1486,7 +1626,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1503,7 +1643,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1520,7 +1660,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -1537,7 +1677,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1553,25 +1693,22 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -1588,7 +1725,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -1605,7 +1742,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1622,7 +1759,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1639,7 +1776,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -1656,46 +1793,46 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="B22" s="2">
         <v>0.7272727272727273</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0.8181818181818181</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>0.7272727272727273</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>0.9090909090909092</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" t="s">
-        <v>68</v>
+      <c r="B26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -1709,7 +1846,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -1723,7 +1860,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1737,7 +1874,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -1751,7 +1888,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -1765,7 +1902,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -1779,7 +1916,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -1793,7 +1930,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B34">
         <v>4</v>
@@ -1807,7 +1944,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -1821,7 +1958,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -1835,7 +1972,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -1849,7 +1986,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -1863,7 +2000,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -1877,7 +2014,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1891,7 +2028,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -1905,7 +2042,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -1919,7 +2056,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -1933,7 +2070,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -1947,7 +2084,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -1961,7 +2098,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -1975,7 +2112,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -1989,7 +2126,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -2002,22 +2139,19 @@
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" t="s">
-        <v>7</v>
-      </c>
-      <c r="B50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" t="s">
-        <v>68</v>
+      <c r="B50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51">
         <v>7</v>
@@ -2031,7 +2165,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52">
         <v>9</v>
@@ -2045,7 +2179,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B53">
         <v>6</v>
@@ -2059,7 +2193,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -2073,7 +2207,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B56">
         <v>22</v>
@@ -2087,43 +2221,43 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57">
+        <v>12</v>
+      </c>
+      <c r="B57" s="2">
         <v>0.7272727272727273</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="2">
         <v>0.6818181818181818</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="2">
         <v>0.9545454545454545</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>2</v>
       </c>
-      <c r="B61" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" t="s">
-        <v>86</v>
+      <c r="B61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B62">
         <v>3</v>
@@ -2137,7 +2271,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -2151,7 +2285,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -2165,7 +2299,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B65">
         <v>3</v>
@@ -2179,7 +2313,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -2193,7 +2327,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -2207,7 +2341,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -2221,7 +2355,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -2235,7 +2369,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -2249,7 +2383,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -2263,7 +2397,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -2277,7 +2411,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B73">
         <v>4</v>
@@ -2291,7 +2425,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B74">
         <v>3</v>
@@ -2304,22 +2438,19 @@
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" t="s">
-        <v>7</v>
-      </c>
-      <c r="B76" t="s">
-        <v>84</v>
-      </c>
-      <c r="C76" t="s">
-        <v>85</v>
-      </c>
-      <c r="D76" t="s">
-        <v>86</v>
+      <c r="B76" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B77">
         <v>4</v>
@@ -2333,7 +2464,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B78">
         <v>9</v>
@@ -2347,7 +2478,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -2361,7 +2492,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -2375,7 +2506,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B82">
         <v>13</v>
@@ -2389,190 +2520,16 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>13</v>
-      </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-      <c r="C83">
+        <v>12</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1</v>
+      </c>
+      <c r="C83" s="2">
         <v>0.9230769230769231</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="2">
         <v>0.8461538461538463</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2590,83 +2547,80 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2683,7 +2637,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2700,24 +2654,24 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2734,19 +2688,19 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2764,7 +2718,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2774,22 +2728,22 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -2806,7 +2760,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -2823,7 +2777,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2840,7 +2794,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -2856,25 +2810,22 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2891,7 +2842,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -2908,7 +2859,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2925,7 +2876,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2942,7 +2893,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -2959,18 +2910,18 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
         <v>0.25</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0.5</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2989,7 +2940,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2999,22 +2950,22 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -3030,25 +2981,22 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3065,7 +3013,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -3082,7 +3030,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3099,7 +3047,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3116,7 +3064,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3133,18 +3081,18 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3155,7 +3103,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3163,7 +3111,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3173,22 +3121,22 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3205,7 +3153,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3222,7 +3170,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3237,38 +3185,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
+    <row r="7" spans="1:5">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3276,16 +3221,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3293,16 +3238,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3310,67 +3255,50 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>0.5</v>
-      </c>
-      <c r="C15">
-        <v>0.5</v>
-      </c>
-      <c r="D15">
-        <v>0.5</v>
-      </c>
-      <c r="E15">
-        <v>0.5</v>
+      <c r="B14" s="2">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.6666666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -3388,7 +3316,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3398,22 +3326,22 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -3430,7 +3358,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -3447,7 +3375,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3463,25 +3391,22 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3498,7 +3423,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3515,7 +3440,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3532,7 +3457,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3549,7 +3474,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -3566,18 +3491,18 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3588,7 +3513,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3596,150 +3521,477 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.7142857142857142</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.2857142857142857</v>
       </c>
     </row>
   </sheetData>
@@ -3748,6 +4000,150 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -3757,29 +4153,29 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
+      <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -3793,7 +4189,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3807,7 +4203,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -3820,22 +4216,19 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3849,7 +4242,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3863,7 +4256,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -3877,7 +4270,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3891,7 +4284,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -3905,15 +4298,15 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
         <v>0.3333333333333333</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>0.6666666666666666</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3922,7 +4315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3932,26 +4325,26 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3962,7 +4355,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -3973,7 +4366,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -3984,7 +4377,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3994,19 +4387,16 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4017,7 +4407,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -4028,7 +4418,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4039,7 +4429,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4050,7 +4440,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -4061,146 +4451,13 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
         <v>0.75</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
+      <c r="C15" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>